<commit_message>
week 4 day 3
</commit_message>
<xml_diff>
--- a/data/Experiment/Physiology_08132025.xlsx
+++ b/data/Experiment/Physiology_08132025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46D34AD-AEB6-8A49-8ECC-6D49C0258CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9927E663-410B-E641-87E4-AA01F309429E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="12900" windowHeight="17140" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="12900" windowHeight="17120" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
   <sheets>
     <sheet name="PIPO" sheetId="1" r:id="rId1"/>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F958DE17-0E59-E849-A835-10176DABDFD5}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="268" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="268" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,55 +657,88 @@
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>9.3000000000000007</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>8.8000000000000007</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>
@@ -718,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E06963-B773-F348-8854-A3523910E721}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A15" zoomScale="275" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,100 +772,160 @@
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="B2">
+        <v>11.1</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B3">
+        <v>8.4</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B4">
+        <v>10.8</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B6">
+        <v>9.4</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B7">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B8">
+        <v>13.3</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="B11">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="B12">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B13">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B14">
+        <v>8.6999999999999993</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B15">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="B21">
+        <v>2.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>